<commit_message>
implemented k merged list
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gillianye/Desktop/resource/leetcode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gillianye/GitHub profile/Data-Structure-Algoritham/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A949A457-0AFF-B34D-83FC-6EF75EBE43B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DD353E-BDC3-134A-AA7F-ADC5E7B0A97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="1780" windowWidth="36800" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3700" yWindow="2280" windowWidth="36560" windowHeight="24020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -974,7 +974,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -985,6 +985,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -992,38 +993,45 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1031,12 +1039,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1044,6 +1054,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1051,18 +1062,21 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1070,8 +1084,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1126,6 +1147,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1168,7 +1201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1194,6 +1227,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1415,8 +1452,8 @@
   </sheetPr>
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2056,10 +2093,10 @@
       <c r="C38" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="16" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2124,10 +2161,10 @@
       <c r="C42" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="16" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2141,10 +2178,10 @@
       <c r="C43" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="16" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2158,10 +2195,10 @@
       <c r="C44" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="16" t="s">
         <v>175</v>
       </c>
     </row>
@@ -2192,10 +2229,10 @@
       <c r="C46" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="16" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2209,10 +2246,10 @@
       <c r="C47" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="27" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2328,10 +2365,10 @@
       <c r="C54" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="27" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2359,13 +2396,13 @@
       <c r="B56" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="27" t="s">
         <v>222</v>
       </c>
     </row>
@@ -2413,10 +2450,10 @@
       <c r="C59" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="16" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2430,10 +2467,10 @@
       <c r="C60" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="16" t="s">
         <v>238</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented merge sort and qucik sort
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions (NeetCode on yt).xlsx
+++ b/Leetcode 75 Questions (NeetCode on yt).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gillianye/GitHub profile/Data-Structure-Algoritham/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DD353E-BDC3-134A-AA7F-ADC5E7B0A97B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C191C290-2FFA-4843-A330-1EF201B6B7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="2280" windowWidth="36560" windowHeight="24020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4060" yWindow="1280" windowWidth="36560" windowHeight="24020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1452,8 +1452,8 @@
   </sheetPr>
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2212,10 +2212,10 @@
       <c r="C45" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="27" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2484,10 +2484,10 @@
       <c r="C61" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="16" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2501,10 +2501,10 @@
       <c r="C62" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="16" t="s">
         <v>247</v>
       </c>
     </row>
@@ -2518,10 +2518,10 @@
       <c r="C63" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="16" t="s">
         <v>251</v>
       </c>
     </row>
@@ -2535,10 +2535,10 @@
       <c r="C64" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="16" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2569,10 +2569,10 @@
       <c r="C66" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="16" t="s">
         <v>263</v>
       </c>
     </row>
@@ -2603,10 +2603,10 @@
       <c r="C68" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="16" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2671,10 +2671,10 @@
       <c r="C72" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D72" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="16" t="s">
         <v>287</v>
       </c>
     </row>

</xml_diff>